<commit_message>
add: pulse modulation ln, spice_sims
</commit_message>
<xml_diff>
--- a/scripting-and-simulations/tooling/stm32_timer.xlsx
+++ b/scripting-and-simulations/tooling/stm32_timer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\00_Lehre\01_Unterrichtsmaterial\03_Embedded_Systems\C-BSc-Embedded-Systems\stm32-tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\00_Lehre\01_Unterrichtsmaterial\03_Embedded_Systems\C-BSc-Embedded-Systems\scripting-and-simulations\tooling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BFD2CB-D3A4-497F-806C-E9D6F34BA5FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0BEDC4-A782-4481-8323-3BB73E7FEB13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,10 +36,10 @@
     <t>Required ARR</t>
   </si>
   <si>
-    <t>Period from Freq.</t>
+    <t>Desired Freq.</t>
   </si>
   <si>
-    <t>Desired Freq.</t>
+    <t>Desired Period</t>
   </si>
 </sst>
 </file>
@@ -377,7 +377,7 @@
   <dimension ref="A2:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,7 +391,7 @@
   <sheetData>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -422,7 +422,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>